<commit_message>
Switch to updated Adafruit_SSD1306 OLED library.
Switch to updated Adafruit_SSD1306 OLED library.   8 lines x 21 chars
</commit_message>
<xml_diff>
--- a/Mav2PThruESP32_pin-table.xlsx
+++ b/Mav2PThruESP32_pin-table.xlsx
@@ -184,7 +184,7 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6111,7 +6111,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6122,7 +6122,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>